<commit_message>
ContentIndexParser: Support for campaigns
</commit_message>
<xml_diff>
--- a/tests/input/example1/content_index.xlsx
+++ b/tests/input/example1/content_index.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="content_index" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="nesteddata" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="my_basic_flow" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="my_template" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="my_campaign" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -46,6 +47,15 @@
     <t xml:space="preserve">status</t>
   </si>
   <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">create_flow</t>
   </si>
   <si>
@@ -58,15 +68,36 @@
     <t xml:space="preserve">row1</t>
   </si>
   <si>
+    <t xml:space="preserve">advanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type1</t>
+  </si>
+  <si>
     <t xml:space="preserve">row2</t>
   </si>
   <si>
+    <t xml:space="preserve">type2</t>
+  </si>
+  <si>
     <t xml:space="preserve">my_basic_flow</t>
   </si>
   <si>
+    <t xml:space="preserve">basic</t>
+  </si>
+  <si>
     <t xml:space="preserve">NestedRowModel</t>
   </si>
   <si>
+    <t xml:space="preserve">create_campaign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my_campaign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My Group</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -119,6 +150,57 @@
   </si>
   <si>
     <t xml:space="preserve">{{custom_field.happy}} and {{custom_field.sad}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delivery_hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relative_to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Seen On</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created On</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
   </si>
 </sst>
 </file>
@@ -193,8 +275,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,10 +301,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -255,41 +341,65 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,10 +407,29 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -321,7 +450,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -332,44 +461,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -401,27 +530,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -453,35 +582,139 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>